<commit_message>
tilføjet Na data fra Na2OSiO2
</commit_message>
<xml_diff>
--- a/data/NaCl_IC_analyse_test.xlsx
+++ b/data/NaCl_IC_analyse_test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{3C0C4C5D-0172-4F0F-BDE4-87CB5391D010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{09BB1CBD-DE27-4126-A8D9-930F319CCE7B}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{3C0C4C5D-0172-4F0F-BDE4-87CB5391D010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{65C504F7-FE96-4131-8CD0-EEF9952DEE7B}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="NaCl" sheetId="1" r:id="rId1"/>
     <sheet name="CaCl2" sheetId="2" r:id="rId2"/>
+    <sheet name="SiO2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
   <si>
     <t>navn</t>
   </si>
@@ -57,11 +58,17 @@
   <si>
     <t>Ca  [mg/l]</t>
   </si>
+  <si>
+    <t>SiO2  [mg/l]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -121,6 +128,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F5B53-D1CD-43A2-82D9-8A2F69E97C05}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,4 +972,268 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AF8B36-B0FD-4CC9-B091-FE33E35F5622}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="C2" s="4">
+        <v>47.6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>60.7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>48.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4">
+        <v>48.3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>52.8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>60.3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4">
+        <v>62.7</v>
+      </c>
+      <c r="C7" s="4">
+        <v>52.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <v>55.5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>24.4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4">
+        <v>63.6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>59.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
+        <v>63.9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>58.9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4">
+        <v>54.7</v>
+      </c>
+      <c r="C11" s="5">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B12" s="4">
+        <v>63.6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>63.9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B13" s="4">
+        <v>63.4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>56.7</v>
+      </c>
+      <c r="C14" s="4">
+        <v>30.1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4">
+        <v>65.3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>68.3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4">
+        <v>51.6</v>
+      </c>
+      <c r="C16" s="4">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B17" s="4">
+        <v>63</v>
+      </c>
+      <c r="C17" s="4">
+        <v>67.2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B18" s="4">
+        <v>52.2</v>
+      </c>
+      <c r="C18" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
charge balance lavet i excel ark.
</commit_message>
<xml_diff>
--- a/data/NaCl_IC_analyse_test.xlsx
+++ b/data/NaCl_IC_analyse_test.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{3C0C4C5D-0172-4F0F-BDE4-87CB5391D010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{65C504F7-FE96-4131-8CD0-EEF9952DEE7B}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="8_{3C0C4C5D-0172-4F0F-BDE4-87CB5391D010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2687AD11-D3DD-41C7-A971-D690A157CAE7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="NaCl" sheetId="1" r:id="rId1"/>
     <sheet name="CaCl2" sheetId="2" r:id="rId2"/>
     <sheet name="SiO2" sheetId="3" r:id="rId3"/>
+    <sheet name="NaCl_Check" sheetId="4" r:id="rId4"/>
+    <sheet name="CaCl2_check" sheetId="5" r:id="rId5"/>
+    <sheet name="SiO2_check" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="26">
   <si>
     <t>navn</t>
   </si>
@@ -61,6 +64,60 @@
   <si>
     <t>SiO2  [mg/l]</t>
   </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>stream</t>
+  </si>
+  <si>
+    <t>Ion mg/L</t>
+  </si>
+  <si>
+    <t>Mw</t>
+  </si>
+  <si>
+    <t>Na+</t>
+  </si>
+  <si>
+    <t>Cl-</t>
+  </si>
+  <si>
+    <t>HCO3-</t>
+  </si>
+  <si>
+    <t>Concentration mM</t>
+  </si>
+  <si>
+    <t>anion</t>
+  </si>
+  <si>
+    <t>cation</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>anion sum</t>
+  </si>
+  <si>
+    <t>Ca++</t>
+  </si>
+  <si>
+    <t>deviation charge</t>
+  </si>
+  <si>
+    <t>Na  +</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SiO2  </t>
+  </si>
+  <si>
+    <t>deviation charge w. SiO2</t>
+  </si>
+  <si>
+    <t>deviation charge w/o. SiO2</t>
+  </si>
 </sst>
 </file>
 
@@ -78,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,8 +148,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -115,11 +190,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -130,6 +333,86 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +730,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E18"/>
+      <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,7 +998,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D18"/>
+      <selection activeCell="B2" sqref="B2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AF8B36-B0FD-4CC9-B091-FE33E35F5622}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1236,4 +1519,3194 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C67C5D-97B1-4C27-815C-706A89013963}">
+  <dimension ref="A1:AP20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1">
+        <v>22.99</v>
+      </c>
+      <c r="D1">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="E1">
+        <v>61.016800000000003</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="43"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="C2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="43"/>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="42">
+        <v>82</v>
+      </c>
+      <c r="D4" s="42">
+        <v>131</v>
+      </c>
+      <c r="E4" s="14">
+        <v>8.4</v>
+      </c>
+      <c r="F4" s="20">
+        <f>C4/$C$1</f>
+        <v>3.5667681600695955</v>
+      </c>
+      <c r="G4" s="20">
+        <f>D4/$D$1</f>
+        <v>3.6953455571227076</v>
+      </c>
+      <c r="H4" s="20">
+        <f>E4/$E$1</f>
+        <v>0.13766700318600777</v>
+      </c>
+      <c r="I4" s="24">
+        <f>F4*1</f>
+        <v>3.5667681600695955</v>
+      </c>
+      <c r="J4" s="24">
+        <f t="shared" ref="J4:K4" si="0">G4*1</f>
+        <v>3.6953455571227076</v>
+      </c>
+      <c r="K4" s="24">
+        <f>H4*1</f>
+        <v>0.13766700318600777</v>
+      </c>
+      <c r="L4" s="24">
+        <f>J4+K4</f>
+        <v>3.8330125603087155</v>
+      </c>
+      <c r="M4" s="47">
+        <f>(((L4)-I4)/I4)*100</f>
+        <v>7.4645838554845954</v>
+      </c>
+      <c r="N4" s="8"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+      <c r="AO4"/>
+      <c r="AP4"/>
+    </row>
+    <row r="5" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="34">
+        <v>77</v>
+      </c>
+      <c r="D5" s="34">
+        <v>117</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="35">
+        <f>C5/$C$1</f>
+        <v>3.3492822966507179</v>
+      </c>
+      <c r="G5" s="35">
+        <f>D5/$D$1</f>
+        <v>3.3004231311706627</v>
+      </c>
+      <c r="H5" s="35">
+        <f t="shared" ref="H5:H20" si="1">E5/$E$1</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="36">
+        <f t="shared" ref="I5:I20" si="2">F5*1</f>
+        <v>3.3492822966507179</v>
+      </c>
+      <c r="J5" s="36">
+        <f t="shared" ref="J5:J20" si="3">G5*1</f>
+        <v>3.3004231311706627</v>
+      </c>
+      <c r="K5" s="36">
+        <f t="shared" ref="K5:K20" si="4">H5*1</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="36">
+        <f t="shared" ref="L5:L20" si="5">J5+K5</f>
+        <v>3.3004231311706627</v>
+      </c>
+      <c r="M5" s="48">
+        <f>(((L5)-I5)/I5)*100</f>
+        <v>-1.4587950836187908</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+      <c r="AN5"/>
+      <c r="AO5"/>
+      <c r="AP5"/>
+    </row>
+    <row r="6" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="25">
+        <v>77</v>
+      </c>
+      <c r="D6" s="25">
+        <v>118</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="28">
+        <f>C6/$C$1</f>
+        <v>3.3492822966507179</v>
+      </c>
+      <c r="G6" s="28">
+        <f>D6/$D$1</f>
+        <v>3.328631875881523</v>
+      </c>
+      <c r="H6" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="29">
+        <f t="shared" si="2"/>
+        <v>3.3492822966507179</v>
+      </c>
+      <c r="J6" s="29">
+        <f t="shared" si="3"/>
+        <v>3.328631875881523</v>
+      </c>
+      <c r="K6" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="29">
+        <f t="shared" si="5"/>
+        <v>3.328631875881523</v>
+      </c>
+      <c r="M6" s="49">
+        <f t="shared" ref="M5:M20" si="6">(((L6)-I6)/I6)*100</f>
+        <v>-0.61656256296596124</v>
+      </c>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+      <c r="AN6"/>
+      <c r="AO6"/>
+      <c r="AP6"/>
+    </row>
+    <row r="7" spans="1:42" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="30">
+        <v>61</v>
+      </c>
+      <c r="D7" s="30">
+        <v>97</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="31">
+        <f>C7/$C$1</f>
+        <v>2.6533275337103088</v>
+      </c>
+      <c r="G7" s="31">
+        <f>D7/$D$1</f>
+        <v>2.7362482369534553</v>
+      </c>
+      <c r="H7" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="2"/>
+        <v>2.6533275337103088</v>
+      </c>
+      <c r="J7" s="32">
+        <f t="shared" si="3"/>
+        <v>2.7362482369534553</v>
+      </c>
+      <c r="K7" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="32">
+        <f t="shared" si="5"/>
+        <v>2.7362482369534553</v>
+      </c>
+      <c r="M7" s="50">
+        <f t="shared" si="6"/>
+        <v>3.1251589632130128</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+      <c r="AN7"/>
+      <c r="AO7"/>
+      <c r="AP7"/>
+    </row>
+    <row r="8" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="34">
+        <v>80</v>
+      </c>
+      <c r="D8" s="34">
+        <v>120</v>
+      </c>
+      <c r="E8" s="12">
+        <v>31</v>
+      </c>
+      <c r="F8" s="35">
+        <f>C8/$C$1</f>
+        <v>3.4797738147020447</v>
+      </c>
+      <c r="G8" s="35">
+        <f>D8/$D$1</f>
+        <v>3.3850493653032436</v>
+      </c>
+      <c r="H8" s="35">
+        <f t="shared" si="1"/>
+        <v>0.50805679747217158</v>
+      </c>
+      <c r="I8" s="36">
+        <f t="shared" si="2"/>
+        <v>3.4797738147020447</v>
+      </c>
+      <c r="J8" s="36">
+        <f t="shared" si="3"/>
+        <v>3.3850493653032436</v>
+      </c>
+      <c r="K8" s="36">
+        <f t="shared" si="4"/>
+        <v>0.50805679747217158</v>
+      </c>
+      <c r="L8" s="36">
+        <f t="shared" si="5"/>
+        <v>3.8931061627754153</v>
+      </c>
+      <c r="M8" s="48">
+        <f t="shared" si="6"/>
+        <v>11.878138352758487</v>
+      </c>
+      <c r="N8" s="8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+    </row>
+    <row r="9" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="25">
+        <v>80</v>
+      </c>
+      <c r="D9" s="25">
+        <v>120</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="28">
+        <f>C9/$C$1</f>
+        <v>3.4797738147020447</v>
+      </c>
+      <c r="G9" s="28">
+        <f>D9/$D$1</f>
+        <v>3.3850493653032436</v>
+      </c>
+      <c r="H9" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="29">
+        <f t="shared" si="2"/>
+        <v>3.4797738147020447</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="3"/>
+        <v>3.3850493653032436</v>
+      </c>
+      <c r="K9" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="29">
+        <f t="shared" si="5"/>
+        <v>3.3850493653032436</v>
+      </c>
+      <c r="M9" s="49">
+        <f t="shared" si="6"/>
+        <v>-2.722143864598046</v>
+      </c>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+      <c r="AN9"/>
+      <c r="AO9"/>
+      <c r="AP9"/>
+    </row>
+    <row r="10" spans="1:42" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40">
+        <v>2</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="30">
+        <v>63</v>
+      </c>
+      <c r="D10" s="30">
+        <v>100</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="31">
+        <f>C10/$C$1</f>
+        <v>2.7403218790778601</v>
+      </c>
+      <c r="G10" s="31">
+        <f>D10/$D$1</f>
+        <v>2.8208744710860363</v>
+      </c>
+      <c r="H10" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="32">
+        <f t="shared" si="2"/>
+        <v>2.7403218790778601</v>
+      </c>
+      <c r="J10" s="32">
+        <f t="shared" si="3"/>
+        <v>2.8208744710860363</v>
+      </c>
+      <c r="K10" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="32">
+        <f t="shared" si="5"/>
+        <v>2.8208744710860363</v>
+      </c>
+      <c r="M10" s="50">
+        <f t="shared" si="6"/>
+        <v>2.9395303020126526</v>
+      </c>
+      <c r="N10" s="8"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AN10"/>
+      <c r="AO10"/>
+      <c r="AP10"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A11" s="33">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="34">
+        <v>85</v>
+      </c>
+      <c r="D11" s="34">
+        <v>127</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="35">
+        <f>C11/$C$1</f>
+        <v>3.6972596781209224</v>
+      </c>
+      <c r="G11" s="35">
+        <f>D11/$D$1</f>
+        <v>3.5825105782792663</v>
+      </c>
+      <c r="H11" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="36">
+        <f t="shared" si="2"/>
+        <v>3.6972596781209224</v>
+      </c>
+      <c r="J11" s="36">
+        <f t="shared" si="3"/>
+        <v>3.5825105782792663</v>
+      </c>
+      <c r="K11" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="36">
+        <f t="shared" si="5"/>
+        <v>3.5825105782792663</v>
+      </c>
+      <c r="M11" s="48">
+        <f t="shared" si="6"/>
+        <v>-3.1036256533643205</v>
+      </c>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="25">
+        <v>85</v>
+      </c>
+      <c r="D12" s="25">
+        <v>125</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="28">
+        <f>C12/$C$1</f>
+        <v>3.6972596781209224</v>
+      </c>
+      <c r="G12" s="28">
+        <f>D12/$D$1</f>
+        <v>3.5260930888575457</v>
+      </c>
+      <c r="H12" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="2"/>
+        <v>3.6972596781209224</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="3"/>
+        <v>3.5260930888575457</v>
+      </c>
+      <c r="K12" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="29">
+        <f t="shared" si="5"/>
+        <v>3.5260930888575457</v>
+      </c>
+      <c r="M12" s="49">
+        <f t="shared" si="6"/>
+        <v>-4.6295528084294473</v>
+      </c>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A13" s="40">
+        <v>3</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="30">
+        <v>66</v>
+      </c>
+      <c r="D13" s="30">
+        <v>105</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="31">
+        <f>C13/$C$1</f>
+        <v>2.8708133971291869</v>
+      </c>
+      <c r="G13" s="31">
+        <f>D13/$D$1</f>
+        <v>2.9619181946403383</v>
+      </c>
+      <c r="H13" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="32">
+        <f t="shared" si="2"/>
+        <v>2.8708133971291869</v>
+      </c>
+      <c r="J13" s="32">
+        <f t="shared" si="3"/>
+        <v>2.9619181946403383</v>
+      </c>
+      <c r="K13" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="32">
+        <f t="shared" si="5"/>
+        <v>2.9619181946403383</v>
+      </c>
+      <c r="M13" s="50">
+        <f t="shared" si="6"/>
+        <v>3.1734837799717739</v>
+      </c>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="34">
+        <v>89</v>
+      </c>
+      <c r="D14" s="34">
+        <v>129</v>
+      </c>
+      <c r="E14" s="12">
+        <v>42</v>
+      </c>
+      <c r="F14" s="35">
+        <f>C14/$C$1</f>
+        <v>3.8712483688560244</v>
+      </c>
+      <c r="G14" s="35">
+        <f>D14/$D$1</f>
+        <v>3.638928067700987</v>
+      </c>
+      <c r="H14" s="35">
+        <f t="shared" si="1"/>
+        <v>0.68833501593003887</v>
+      </c>
+      <c r="I14" s="36">
+        <f t="shared" si="2"/>
+        <v>3.8712483688560244</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" si="3"/>
+        <v>3.638928067700987</v>
+      </c>
+      <c r="K14" s="36">
+        <f t="shared" si="4"/>
+        <v>0.68833501593003887</v>
+      </c>
+      <c r="L14" s="36">
+        <f t="shared" si="5"/>
+        <v>4.327263083631026</v>
+      </c>
+      <c r="M14" s="48">
+        <f t="shared" si="6"/>
+        <v>11.779526171547513</v>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+    </row>
+    <row r="15" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38">
+        <v>3.5</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="25">
+        <v>88</v>
+      </c>
+      <c r="D15" s="25">
+        <v>128</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="28">
+        <f>C15/$C$1</f>
+        <v>3.8277511961722492</v>
+      </c>
+      <c r="G15" s="28">
+        <f>D15/$D$1</f>
+        <v>3.6107193229901267</v>
+      </c>
+      <c r="H15" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="29">
+        <f t="shared" si="2"/>
+        <v>3.8277511961722492</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" si="3"/>
+        <v>3.6107193229901267</v>
+      </c>
+      <c r="K15" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="29">
+        <f t="shared" si="5"/>
+        <v>3.6107193229901267</v>
+      </c>
+      <c r="M15" s="49">
+        <f t="shared" si="6"/>
+        <v>-5.6699576868829515</v>
+      </c>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AN15"/>
+      <c r="AO15"/>
+      <c r="AP15"/>
+    </row>
+    <row r="16" spans="1:42" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="40">
+        <v>3.5</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="30">
+        <v>68</v>
+      </c>
+      <c r="D16" s="30">
+        <v>109</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="31">
+        <f>C16/$C$1</f>
+        <v>2.9578077424967377</v>
+      </c>
+      <c r="G16" s="31">
+        <f>D16/$D$1</f>
+        <v>3.0747531734837796</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="32">
+        <f t="shared" si="2"/>
+        <v>2.9578077424967377</v>
+      </c>
+      <c r="J16" s="32">
+        <f t="shared" si="3"/>
+        <v>3.0747531734837796</v>
+      </c>
+      <c r="K16" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="32">
+        <f t="shared" si="5"/>
+        <v>3.0747531734837796</v>
+      </c>
+      <c r="M16" s="50">
+        <f t="shared" si="6"/>
+        <v>3.9537874388119025</v>
+      </c>
+      <c r="N16" s="8"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AN16"/>
+      <c r="AO16"/>
+      <c r="AP16"/>
+    </row>
+    <row r="17" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="34">
+        <v>91</v>
+      </c>
+      <c r="D17" s="34">
+        <v>134</v>
+      </c>
+      <c r="E17" s="12">
+        <v>48</v>
+      </c>
+      <c r="F17" s="35">
+        <f>C17/$C$1</f>
+        <v>3.9582427142235757</v>
+      </c>
+      <c r="G17" s="35">
+        <f>D17/$D$1</f>
+        <v>3.779971791255289</v>
+      </c>
+      <c r="H17" s="35">
+        <f t="shared" si="1"/>
+        <v>0.78666858963433017</v>
+      </c>
+      <c r="I17" s="36">
+        <f t="shared" si="2"/>
+        <v>3.9582427142235757</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="3"/>
+        <v>3.779971791255289</v>
+      </c>
+      <c r="K17" s="36">
+        <f t="shared" si="4"/>
+        <v>0.78666858963433017</v>
+      </c>
+      <c r="L17" s="36">
+        <f t="shared" si="5"/>
+        <v>4.566640380889619</v>
+      </c>
+      <c r="M17" s="48">
+        <f t="shared" si="6"/>
+        <v>15.370398194123446</v>
+      </c>
+      <c r="N17" s="8"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AN17"/>
+      <c r="AO17"/>
+      <c r="AP17"/>
+    </row>
+    <row r="18" spans="1:42" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="40">
+        <v>4</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="30">
+        <v>72</v>
+      </c>
+      <c r="D18" s="30">
+        <v>113</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="31">
+        <f>C18/$C$1</f>
+        <v>3.1317964332318402</v>
+      </c>
+      <c r="G18" s="31">
+        <f>D18/$D$1</f>
+        <v>3.1875881523272214</v>
+      </c>
+      <c r="H18" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="32">
+        <f t="shared" si="2"/>
+        <v>3.1317964332318402</v>
+      </c>
+      <c r="J18" s="32">
+        <f t="shared" si="3"/>
+        <v>3.1875881523272214</v>
+      </c>
+      <c r="K18" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="32">
+        <f t="shared" si="5"/>
+        <v>3.1875881523272214</v>
+      </c>
+      <c r="M18" s="50">
+        <f t="shared" si="6"/>
+        <v>1.7814605861150179</v>
+      </c>
+      <c r="N18" s="8"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+      <c r="AP18"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A19" s="33">
+        <v>4.5</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="34">
+        <v>86</v>
+      </c>
+      <c r="D19" s="34">
+        <v>127</v>
+      </c>
+      <c r="E19" s="13">
+        <v>43</v>
+      </c>
+      <c r="F19" s="35">
+        <f>C19/$C$1</f>
+        <v>3.740756850804698</v>
+      </c>
+      <c r="G19" s="35">
+        <f>D19/$D$1</f>
+        <v>3.5825105782792663</v>
+      </c>
+      <c r="H19" s="35">
+        <f t="shared" si="1"/>
+        <v>0.70472394488075407</v>
+      </c>
+      <c r="I19" s="36">
+        <f t="shared" si="2"/>
+        <v>3.740756850804698</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="3"/>
+        <v>3.5825105782792663</v>
+      </c>
+      <c r="K19" s="36">
+        <f t="shared" si="4"/>
+        <v>0.70472394488075407</v>
+      </c>
+      <c r="L19" s="36">
+        <f t="shared" si="5"/>
+        <v>4.28723452316002</v>
+      </c>
+      <c r="M19" s="48">
+        <f t="shared" si="6"/>
+        <v>14.608746148196339</v>
+      </c>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A20" s="40">
+        <v>4.5</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="30">
+        <v>60</v>
+      </c>
+      <c r="D20" s="30">
+        <v>96</v>
+      </c>
+      <c r="E20" s="13">
+        <v>15</v>
+      </c>
+      <c r="F20" s="31">
+        <f>C20/$C$1</f>
+        <v>2.6098303610265337</v>
+      </c>
+      <c r="G20" s="31">
+        <f>D20/$D$1</f>
+        <v>2.708039492242595</v>
+      </c>
+      <c r="H20" s="31">
+        <f t="shared" si="1"/>
+        <v>0.24583393426072817</v>
+      </c>
+      <c r="I20" s="32">
+        <f t="shared" si="2"/>
+        <v>2.6098303610265337</v>
+      </c>
+      <c r="J20" s="32">
+        <f t="shared" si="3"/>
+        <v>2.708039492242595</v>
+      </c>
+      <c r="K20" s="32">
+        <f t="shared" si="4"/>
+        <v>0.24583393426072817</v>
+      </c>
+      <c r="L20" s="32">
+        <f t="shared" si="5"/>
+        <v>2.9538734265033231</v>
+      </c>
+      <c r="M20" s="50">
+        <f t="shared" si="6"/>
+        <v>13.182583458852312</v>
+      </c>
+      <c r="N20" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9206B6-6E8E-47B4-864A-F5ED17145FD2}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="D1">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="E1">
+        <v>61.016800000000003</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="43"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="43"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>119</v>
+      </c>
+      <c r="D4" s="3">
+        <v>216</v>
+      </c>
+      <c r="E4" s="11">
+        <v>6</v>
+      </c>
+      <c r="F4" s="20">
+        <f>C4/$C$1</f>
+        <v>2.9692100404211783</v>
+      </c>
+      <c r="G4" s="20">
+        <f>D4/$D$1</f>
+        <v>6.0930888575458386</v>
+      </c>
+      <c r="H4" s="20">
+        <f>E4/$E$1</f>
+        <v>9.8333573704291272E-2</v>
+      </c>
+      <c r="I4" s="24">
+        <f>F4*2</f>
+        <v>5.9384200808423566</v>
+      </c>
+      <c r="J4" s="24">
+        <f t="shared" ref="J4:K19" si="0">G4*1</f>
+        <v>6.0930888575458386</v>
+      </c>
+      <c r="K4" s="24">
+        <f>H4*1</f>
+        <v>9.8333573704291272E-2</v>
+      </c>
+      <c r="L4" s="24">
+        <f>J4+K4</f>
+        <v>6.19142243125013</v>
+      </c>
+      <c r="M4" s="47">
+        <f>(((L4)-I4)/I4)*100</f>
+        <v>4.2604320166566154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>118</v>
+      </c>
+      <c r="D5" s="3">
+        <v>223</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="35">
+        <f>C5/$C$1</f>
+        <v>2.9442586955436898</v>
+      </c>
+      <c r="G5" s="35">
+        <f>D5/$D$1</f>
+        <v>6.2905500705218609</v>
+      </c>
+      <c r="H5" s="20">
+        <f t="shared" ref="H5:H20" si="1">E5/$E$1</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="24">
+        <f t="shared" ref="I5:I20" si="2">F5*2</f>
+        <v>5.8885173910873796</v>
+      </c>
+      <c r="J5" s="36">
+        <f t="shared" si="0"/>
+        <v>6.2905500705218609</v>
+      </c>
+      <c r="K5" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="36">
+        <f t="shared" ref="L5:L20" si="3">J5+K5</f>
+        <v>6.2905500705218609</v>
+      </c>
+      <c r="M5" s="48">
+        <f>(((L5)-I5)/I5)*100</f>
+        <v>6.8274007315148904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>115</v>
+      </c>
+      <c r="D6" s="3">
+        <v>220</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="28">
+        <f>C6/$C$1</f>
+        <v>2.8694046609112229</v>
+      </c>
+      <c r="G6" s="28">
+        <f>D6/$D$1</f>
+        <v>6.2059238363892799</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="24">
+        <f t="shared" si="2"/>
+        <v>5.7388093218224459</v>
+      </c>
+      <c r="J6" s="29">
+        <f t="shared" si="0"/>
+        <v>6.2059238363892799</v>
+      </c>
+      <c r="K6" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="29">
+        <f t="shared" si="3"/>
+        <v>6.2059238363892799</v>
+      </c>
+      <c r="M6" s="49">
+        <f t="shared" ref="M6:M20" si="4">(((L6)-I6)/I6)*100</f>
+        <v>8.1395719629606855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3">
+        <v>106</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="31">
+        <f>C7/$C$1</f>
+        <v>1.1228105194870002</v>
+      </c>
+      <c r="G7" s="31">
+        <f>D7/$D$1</f>
+        <v>2.9901269393511987</v>
+      </c>
+      <c r="H7" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="24">
+        <f t="shared" si="2"/>
+        <v>2.2456210389740003</v>
+      </c>
+      <c r="J7" s="32">
+        <f t="shared" si="0"/>
+        <v>2.9901269393511987</v>
+      </c>
+      <c r="K7" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="32">
+        <f t="shared" si="3"/>
+        <v>2.9901269393511987</v>
+      </c>
+      <c r="M7" s="50">
+        <f t="shared" si="4"/>
+        <v>33.153674972574841</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3">
+        <v>132</v>
+      </c>
+      <c r="D8" s="3">
+        <v>246</v>
+      </c>
+      <c r="E8" s="12">
+        <v>15</v>
+      </c>
+      <c r="F8" s="35">
+        <f>C8/$C$1</f>
+        <v>3.2935775238285343</v>
+      </c>
+      <c r="G8" s="35">
+        <f>D8/$D$1</f>
+        <v>6.9393511988716501</v>
+      </c>
+      <c r="H8" s="20">
+        <f t="shared" si="1"/>
+        <v>0.24583393426072817</v>
+      </c>
+      <c r="I8" s="24">
+        <f t="shared" si="2"/>
+        <v>6.5871550476570686</v>
+      </c>
+      <c r="J8" s="36">
+        <f t="shared" si="0"/>
+        <v>6.9393511988716501</v>
+      </c>
+      <c r="K8" s="36">
+        <f t="shared" si="0"/>
+        <v>0.24583393426072817</v>
+      </c>
+      <c r="L8" s="36">
+        <f t="shared" si="3"/>
+        <v>7.1851851331323786</v>
+      </c>
+      <c r="M8" s="48">
+        <f t="shared" si="4"/>
+        <v>9.0787309718482856</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>133</v>
+      </c>
+      <c r="D9" s="3">
+        <v>248</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="28">
+        <f>C9/$C$1</f>
+        <v>3.3185288687060228</v>
+      </c>
+      <c r="G9" s="28">
+        <f>D9/$D$1</f>
+        <v>6.9957686882933707</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
+        <f t="shared" si="2"/>
+        <v>6.6370577374120456</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="0"/>
+        <v>6.9957686882933707</v>
+      </c>
+      <c r="K9" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="29">
+        <f t="shared" si="3"/>
+        <v>6.9957686882933707</v>
+      </c>
+      <c r="M9" s="49">
+        <f t="shared" si="4"/>
+        <v>5.4046682291059209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3">
+        <v>109</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="31">
+        <f>C10/$C$1</f>
+        <v>1.2226158989969558</v>
+      </c>
+      <c r="G10" s="31">
+        <f>D10/$D$1</f>
+        <v>3.0747531734837796</v>
+      </c>
+      <c r="H10" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="24">
+        <f t="shared" si="2"/>
+        <v>2.4452317979939115</v>
+      </c>
+      <c r="J10" s="32">
+        <f t="shared" si="0"/>
+        <v>3.0747531734837796</v>
+      </c>
+      <c r="K10" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="32">
+        <f t="shared" si="3"/>
+        <v>3.0747531734837796</v>
+      </c>
+      <c r="M10" s="50">
+        <f t="shared" si="4"/>
+        <v>25.744854782533611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>150</v>
+      </c>
+      <c r="D11" s="3">
+        <v>277</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="35">
+        <f>C11/$C$1</f>
+        <v>3.7427017316233342</v>
+      </c>
+      <c r="G11" s="35">
+        <f>D11/$D$1</f>
+        <v>7.813822284908321</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="24">
+        <f t="shared" si="2"/>
+        <v>7.4854034632466684</v>
+      </c>
+      <c r="J11" s="36">
+        <f t="shared" si="0"/>
+        <v>7.813822284908321</v>
+      </c>
+      <c r="K11" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="36">
+        <f t="shared" si="3"/>
+        <v>7.813822284908321</v>
+      </c>
+      <c r="M11" s="48">
+        <f t="shared" si="4"/>
+        <v>4.3874565115185709</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>150</v>
+      </c>
+      <c r="D12" s="3">
+        <v>265</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="28">
+        <f>C12/$C$1</f>
+        <v>3.7427017316233342</v>
+      </c>
+      <c r="G12" s="28">
+        <f>D12/$D$1</f>
+        <v>7.4753173483779962</v>
+      </c>
+      <c r="H12" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="24">
+        <f t="shared" si="2"/>
+        <v>7.4854034632466684</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="0"/>
+        <v>7.4753173483779962</v>
+      </c>
+      <c r="K12" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="29">
+        <f t="shared" si="3"/>
+        <v>7.4753173483779962</v>
+      </c>
+      <c r="M12" s="49">
+        <f t="shared" si="4"/>
+        <v>-0.13474377056888107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>54</v>
+      </c>
+      <c r="D13" s="3">
+        <v>121</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="31">
+        <f>C13/$C$1</f>
+        <v>1.3473726233844003</v>
+      </c>
+      <c r="G13" s="31">
+        <f>D13/$D$1</f>
+        <v>3.413258110014104</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="24">
+        <f t="shared" si="2"/>
+        <v>2.6947452467688007</v>
+      </c>
+      <c r="J13" s="32">
+        <f t="shared" si="0"/>
+        <v>3.413258110014104</v>
+      </c>
+      <c r="K13" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="32">
+        <f t="shared" si="3"/>
+        <v>3.413258110014104</v>
+      </c>
+      <c r="M13" s="50">
+        <f t="shared" si="4"/>
+        <v>26.663480123282657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <v>163</v>
+      </c>
+      <c r="D14" s="3">
+        <v>280</v>
+      </c>
+      <c r="E14" s="12">
+        <v>18</v>
+      </c>
+      <c r="F14" s="35">
+        <f>C14/$C$1</f>
+        <v>4.0670692150306902</v>
+      </c>
+      <c r="G14" s="35">
+        <f>D14/$D$1</f>
+        <v>7.8984485190409019</v>
+      </c>
+      <c r="H14" s="20">
+        <f t="shared" si="1"/>
+        <v>0.29500072111287379</v>
+      </c>
+      <c r="I14" s="24">
+        <f t="shared" si="2"/>
+        <v>8.1341384300613804</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" si="0"/>
+        <v>7.8984485190409019</v>
+      </c>
+      <c r="K14" s="36">
+        <f t="shared" si="0"/>
+        <v>0.29500072111287379</v>
+      </c>
+      <c r="L14" s="36">
+        <f t="shared" si="3"/>
+        <v>8.1934492401537753</v>
+      </c>
+      <c r="M14" s="48">
+        <f t="shared" si="4"/>
+        <v>0.72915909413589064</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3">
+        <v>166</v>
+      </c>
+      <c r="D15" s="3">
+        <v>302</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="28">
+        <f>C15/$C$1</f>
+        <v>4.1419232496631562</v>
+      </c>
+      <c r="G15" s="28">
+        <f>D15/$D$1</f>
+        <v>8.5190409026798299</v>
+      </c>
+      <c r="H15" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="24">
+        <f t="shared" si="2"/>
+        <v>8.2838464993263123</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" si="0"/>
+        <v>8.5190409026798299</v>
+      </c>
+      <c r="K15" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="29">
+        <f t="shared" si="3"/>
+        <v>8.5190409026798299</v>
+      </c>
+      <c r="M15" s="49">
+        <f t="shared" si="4"/>
+        <v>2.8391931619283977</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>56</v>
+      </c>
+      <c r="D16" s="3">
+        <v>119</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="31">
+        <f>C16/$C$1</f>
+        <v>1.397275313139378</v>
+      </c>
+      <c r="G16" s="31">
+        <f>D16/$D$1</f>
+        <v>3.3568406205923833</v>
+      </c>
+      <c r="H16" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="24">
+        <f t="shared" si="2"/>
+        <v>2.7945506262787561</v>
+      </c>
+      <c r="J16" s="32">
+        <f t="shared" si="0"/>
+        <v>3.3568406205923833</v>
+      </c>
+      <c r="K16" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="32">
+        <f t="shared" si="3"/>
+        <v>3.3568406205923833</v>
+      </c>
+      <c r="M16" s="50">
+        <f t="shared" si="4"/>
+        <v>20.120944992947816</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>184</v>
+      </c>
+      <c r="D17" s="3">
+        <v>329</v>
+      </c>
+      <c r="E17" s="12">
+        <v>20</v>
+      </c>
+      <c r="F17" s="35">
+        <f>C17/$C$1</f>
+        <v>4.5910474574579565</v>
+      </c>
+      <c r="G17" s="35">
+        <f>D17/$D$1</f>
+        <v>9.2806770098730595</v>
+      </c>
+      <c r="H17" s="20">
+        <f t="shared" si="1"/>
+        <v>0.32777857901430424</v>
+      </c>
+      <c r="I17" s="24">
+        <f t="shared" si="2"/>
+        <v>9.182094914915913</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="0"/>
+        <v>9.2806770098730595</v>
+      </c>
+      <c r="K17" s="36">
+        <f t="shared" si="0"/>
+        <v>0.32777857901430424</v>
+      </c>
+      <c r="L17" s="36">
+        <f t="shared" si="3"/>
+        <v>9.6084555888873631</v>
+      </c>
+      <c r="M17" s="48">
+        <f t="shared" si="4"/>
+        <v>4.6433921444097219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>61</v>
+      </c>
+      <c r="D18" s="3">
+        <v>126</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="31">
+        <f>C18/$C$1</f>
+        <v>1.5220320375268226</v>
+      </c>
+      <c r="G18" s="31">
+        <f>D18/$D$1</f>
+        <v>3.554301833568406</v>
+      </c>
+      <c r="H18" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
+        <f t="shared" si="2"/>
+        <v>3.0440640750536452</v>
+      </c>
+      <c r="J18" s="32">
+        <f t="shared" si="0"/>
+        <v>3.554301833568406</v>
+      </c>
+      <c r="K18" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="32">
+        <f t="shared" si="3"/>
+        <v>3.554301833568406</v>
+      </c>
+      <c r="M18" s="50">
+        <f t="shared" si="4"/>
+        <v>16.761728594880807</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>178</v>
+      </c>
+      <c r="D19" s="3">
+        <v>320</v>
+      </c>
+      <c r="E19" s="12">
+        <v>20</v>
+      </c>
+      <c r="F19" s="35">
+        <f>C19/$C$1</f>
+        <v>4.4413393881930237</v>
+      </c>
+      <c r="G19" s="35">
+        <f>D19/$D$1</f>
+        <v>9.0267983074753158</v>
+      </c>
+      <c r="H19" s="20">
+        <f t="shared" si="1"/>
+        <v>0.32777857901430424</v>
+      </c>
+      <c r="I19" s="24">
+        <f t="shared" si="2"/>
+        <v>8.8826787763860473</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="0"/>
+        <v>9.0267983074753158</v>
+      </c>
+      <c r="K19" s="36">
+        <f t="shared" si="0"/>
+        <v>0.32777857901430424</v>
+      </c>
+      <c r="L19" s="36">
+        <f t="shared" si="3"/>
+        <v>9.3545768864896193</v>
+      </c>
+      <c r="M19" s="48">
+        <f t="shared" si="4"/>
+        <v>5.3125652968345385</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3">
+        <v>48</v>
+      </c>
+      <c r="D20" s="3">
+        <v>111</v>
+      </c>
+      <c r="E20" s="14">
+        <v>7.8</v>
+      </c>
+      <c r="F20" s="31">
+        <f>C20/$C$1</f>
+        <v>1.197664554119467</v>
+      </c>
+      <c r="G20" s="31">
+        <f>D20/$D$1</f>
+        <v>3.1311706629055003</v>
+      </c>
+      <c r="H20" s="20">
+        <f t="shared" si="1"/>
+        <v>0.12783364581557866</v>
+      </c>
+      <c r="I20" s="24">
+        <f t="shared" si="2"/>
+        <v>2.3953291082389341</v>
+      </c>
+      <c r="J20" s="32">
+        <f t="shared" ref="I5:K20" si="5">G20*1</f>
+        <v>3.1311706629055003</v>
+      </c>
+      <c r="K20" s="32">
+        <f t="shared" si="5"/>
+        <v>0.12783364581557866</v>
+      </c>
+      <c r="L20" s="32">
+        <f t="shared" si="3"/>
+        <v>3.2590043087210789</v>
+      </c>
+      <c r="M20" s="50">
+        <f t="shared" si="4"/>
+        <v>36.056640296795209</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401685D4-8829-42D7-BB4A-E3F815791FE0}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1">
+        <v>22.99</v>
+      </c>
+      <c r="D1">
+        <v>60.08</v>
+      </c>
+      <c r="E1">
+        <v>61.016800000000003</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="F2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>47.6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="E4" s="11">
+        <v>126</v>
+      </c>
+      <c r="F4" s="31">
+        <f>C4/$C$1</f>
+        <v>2.0704654197477166</v>
+      </c>
+      <c r="G4" s="31">
+        <f>D4/$D$1</f>
+        <v>1.0669107856191744</v>
+      </c>
+      <c r="H4" s="31">
+        <f>E4/$E$1</f>
+        <v>2.0650050477901165</v>
+      </c>
+      <c r="I4" s="32">
+        <f>F4*1</f>
+        <v>2.0704654197477166</v>
+      </c>
+      <c r="J4" s="32">
+        <f>G4*1</f>
+        <v>1.0669107856191744</v>
+      </c>
+      <c r="K4" s="32">
+        <f>H4*1</f>
+        <v>2.0650050477901165</v>
+      </c>
+      <c r="L4" s="32">
+        <f>J4+K4</f>
+        <v>3.1319158334092911</v>
+      </c>
+      <c r="M4" s="45">
+        <f>(((L4)-I4)/I4)*100</f>
+        <v>51.266271029578981</v>
+      </c>
+      <c r="N4" s="45">
+        <f>(((K4)-I4)/I4)*100</f>
+        <v>-0.2637267884563565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>48.5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>60.7</v>
+      </c>
+      <c r="E5" s="12">
+        <v>141</v>
+      </c>
+      <c r="F5" s="31">
+        <f t="shared" ref="F5:F20" si="0">C5/$C$1</f>
+        <v>2.1096128751631147</v>
+      </c>
+      <c r="G5" s="31">
+        <f t="shared" ref="G5:G20" si="1">D5/$D$1</f>
+        <v>1.0103195739014648</v>
+      </c>
+      <c r="H5" s="31">
+        <f t="shared" ref="H5:H20" si="2">E5/$E$1</f>
+        <v>2.310838982050845</v>
+      </c>
+      <c r="I5" s="36">
+        <f t="shared" ref="I5:K20" si="3">F5*1</f>
+        <v>2.1096128751631147</v>
+      </c>
+      <c r="J5" s="36">
+        <f t="shared" ref="J4:K19" si="4">G5*1</f>
+        <v>1.0103195739014648</v>
+      </c>
+      <c r="K5" s="37">
+        <f t="shared" si="4"/>
+        <v>2.310838982050845</v>
+      </c>
+      <c r="L5" s="32">
+        <f t="shared" ref="L5:L20" si="5">J5+K5</f>
+        <v>3.3211585559523096</v>
+      </c>
+      <c r="M5" s="45">
+        <f>(((L5)-I5)/I5)*100</f>
+        <v>57.429763301739357</v>
+      </c>
+      <c r="N5" s="45">
+        <f t="shared" ref="N5:N20" si="6">(((K5)-I5)/I5)*100</f>
+        <v>9.5385323656678764</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>48.3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>62</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="31">
+        <f t="shared" si="0"/>
+        <v>2.1009134406263592</v>
+      </c>
+      <c r="G6" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0319573901464714</v>
+      </c>
+      <c r="H6" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="29">
+        <f t="shared" si="3"/>
+        <v>2.1009134406263592</v>
+      </c>
+      <c r="J6" s="29">
+        <f t="shared" si="4"/>
+        <v>1.0319573901464714</v>
+      </c>
+      <c r="K6" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="32">
+        <f t="shared" si="5"/>
+        <v>1.0319573901464714</v>
+      </c>
+      <c r="M6" s="45">
+        <f t="shared" ref="M6:N20" si="7">(((L6)-I6)/I6)*100</f>
+        <v>-50.880537475222823</v>
+      </c>
+      <c r="N6" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>52.8</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="31">
+        <f t="shared" si="0"/>
+        <v>0.91779034362766432</v>
+      </c>
+      <c r="G7" s="31">
+        <f t="shared" si="1"/>
+        <v>0.87882822902796265</v>
+      </c>
+      <c r="H7" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="3"/>
+        <v>0.91779034362766432</v>
+      </c>
+      <c r="J7" s="32">
+        <f t="shared" si="4"/>
+        <v>0.87882822902796265</v>
+      </c>
+      <c r="K7" s="41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="32">
+        <f t="shared" si="5"/>
+        <v>0.87882822902796265</v>
+      </c>
+      <c r="M7" s="45">
+        <f t="shared" si="7"/>
+        <v>-4.2452086002234184</v>
+      </c>
+      <c r="N7" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5">
+        <v>53</v>
+      </c>
+      <c r="D8" s="4">
+        <v>60.3</v>
+      </c>
+      <c r="E8" s="12">
+        <v>157</v>
+      </c>
+      <c r="F8" s="31">
+        <f t="shared" si="0"/>
+        <v>2.3053501522401048</v>
+      </c>
+      <c r="G8" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0036617842876165</v>
+      </c>
+      <c r="H8" s="31">
+        <f t="shared" si="2"/>
+        <v>2.5730618452622882</v>
+      </c>
+      <c r="I8" s="36">
+        <f t="shared" si="3"/>
+        <v>2.3053501522401048</v>
+      </c>
+      <c r="J8" s="36">
+        <f t="shared" si="4"/>
+        <v>1.0036617842876165</v>
+      </c>
+      <c r="K8" s="37">
+        <f t="shared" si="4"/>
+        <v>2.5730618452622882</v>
+      </c>
+      <c r="L8" s="32">
+        <f t="shared" si="5"/>
+        <v>3.576723629549905</v>
+      </c>
+      <c r="M8" s="45">
+        <f t="shared" si="7"/>
+        <v>55.148823100664721</v>
+      </c>
+      <c r="N8" s="45">
+        <f t="shared" si="6"/>
+        <v>11.612626080339616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>52.7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>62.7</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="31">
+        <f t="shared" si="0"/>
+        <v>2.2923010004349722</v>
+      </c>
+      <c r="G9" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0436085219707059</v>
+      </c>
+      <c r="H9" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="29">
+        <f t="shared" si="3"/>
+        <v>2.2923010004349722</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="4"/>
+        <v>1.0436085219707059</v>
+      </c>
+      <c r="K9" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="32">
+        <f t="shared" si="5"/>
+        <v>1.0436085219707059</v>
+      </c>
+      <c r="M9" s="45">
+        <f t="shared" si="7"/>
+        <v>-54.473320834712482</v>
+      </c>
+      <c r="N9" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
+        <v>24.4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>55.5</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="31">
+        <f t="shared" si="0"/>
+        <v>1.0613310134841236</v>
+      </c>
+      <c r="G10" s="31">
+        <f t="shared" si="1"/>
+        <v>0.92376830892143813</v>
+      </c>
+      <c r="H10" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="32">
+        <f t="shared" si="3"/>
+        <v>1.0613310134841236</v>
+      </c>
+      <c r="J10" s="32">
+        <f t="shared" si="4"/>
+        <v>0.92376830892143813</v>
+      </c>
+      <c r="K10" s="41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="32">
+        <f t="shared" si="5"/>
+        <v>0.92376830892143813</v>
+      </c>
+      <c r="M10" s="45">
+        <f t="shared" si="7"/>
+        <v>-12.961338434000572</v>
+      </c>
+      <c r="N10" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>59.5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>63.6</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="31">
+        <f t="shared" si="0"/>
+        <v>2.5880817746846456</v>
+      </c>
+      <c r="G11" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0585885486018642</v>
+      </c>
+      <c r="H11" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="36">
+        <f t="shared" si="3"/>
+        <v>2.5880817746846456</v>
+      </c>
+      <c r="J11" s="36">
+        <f t="shared" si="4"/>
+        <v>1.0585885486018642</v>
+      </c>
+      <c r="K11" s="37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="32">
+        <f t="shared" si="5"/>
+        <v>1.0585885486018642</v>
+      </c>
+      <c r="M11" s="45">
+        <f t="shared" si="7"/>
+        <v>-59.097561794358221</v>
+      </c>
+      <c r="N11" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <v>58.9</v>
+      </c>
+      <c r="D12" s="4">
+        <v>63.9</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="31">
+        <f t="shared" si="0"/>
+        <v>2.5619834710743801</v>
+      </c>
+      <c r="G12" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0635818908122503</v>
+      </c>
+      <c r="H12" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="3"/>
+        <v>2.5619834710743801</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="4"/>
+        <v>1.0635818908122503</v>
+      </c>
+      <c r="K12" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="32">
+        <f t="shared" si="5"/>
+        <v>1.0635818908122503</v>
+      </c>
+      <c r="M12" s="45">
+        <f t="shared" si="7"/>
+        <v>-58.485997165070224</v>
+      </c>
+      <c r="N12" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4">
+        <v>54.7</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="31">
+        <f t="shared" si="0"/>
+        <v>1.17442366246194</v>
+      </c>
+      <c r="G13" s="31">
+        <f t="shared" si="1"/>
+        <v>0.9104527296937418</v>
+      </c>
+      <c r="H13" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="32">
+        <f t="shared" si="3"/>
+        <v>1.17442366246194</v>
+      </c>
+      <c r="J13" s="32">
+        <f t="shared" si="4"/>
+        <v>0.9104527296937418</v>
+      </c>
+      <c r="K13" s="41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="32">
+        <f t="shared" si="5"/>
+        <v>0.9104527296937418</v>
+      </c>
+      <c r="M13" s="45">
+        <f t="shared" si="7"/>
+        <v>-22.476636090151391</v>
+      </c>
+      <c r="N13" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>63.9</v>
+      </c>
+      <c r="D14" s="4">
+        <v>63.6</v>
+      </c>
+      <c r="E14" s="4">
+        <v>196</v>
+      </c>
+      <c r="F14" s="31">
+        <f t="shared" si="0"/>
+        <v>2.7794693344932582</v>
+      </c>
+      <c r="G14" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0585885486018642</v>
+      </c>
+      <c r="H14" s="31">
+        <f t="shared" si="2"/>
+        <v>3.2122300743401815</v>
+      </c>
+      <c r="I14" s="36">
+        <f t="shared" si="3"/>
+        <v>2.7794693344932582</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" si="4"/>
+        <v>1.0585885486018642</v>
+      </c>
+      <c r="K14" s="37">
+        <f t="shared" si="4"/>
+        <v>3.2122300743401815</v>
+      </c>
+      <c r="L14" s="32">
+        <f t="shared" si="5"/>
+        <v>4.2708186229420457</v>
+      </c>
+      <c r="M14" s="45">
+        <f t="shared" si="7"/>
+        <v>53.655900064847607</v>
+      </c>
+      <c r="N14" s="45">
+        <f t="shared" si="6"/>
+        <v>15.569905178530149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="D15" s="4">
+        <v>63.4</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="31">
+        <f t="shared" si="0"/>
+        <v>2.8186167899086558</v>
+      </c>
+      <c r="G15" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0552596537949401</v>
+      </c>
+      <c r="H15" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="29">
+        <f t="shared" si="3"/>
+        <v>2.8186167899086558</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" si="4"/>
+        <v>1.0552596537949401</v>
+      </c>
+      <c r="K15" s="39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="32">
+        <f t="shared" si="5"/>
+        <v>1.0552596537949401</v>
+      </c>
+      <c r="M15" s="45">
+        <f t="shared" si="7"/>
+        <v>-62.561081109960384</v>
+      </c>
+      <c r="N15" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>30.1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>56.7</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="31">
+        <f t="shared" si="0"/>
+        <v>1.3092648977816443</v>
+      </c>
+      <c r="G16" s="31">
+        <f t="shared" si="1"/>
+        <v>0.94374167776298279</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="32">
+        <f t="shared" si="3"/>
+        <v>1.3092648977816443</v>
+      </c>
+      <c r="J16" s="32">
+        <f t="shared" si="4"/>
+        <v>0.94374167776298279</v>
+      </c>
+      <c r="K16" s="41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="32">
+        <f t="shared" si="5"/>
+        <v>0.94374167776298279</v>
+      </c>
+      <c r="M16" s="45">
+        <f t="shared" si="7"/>
+        <v>-27.918202087139626</v>
+      </c>
+      <c r="N16" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4">
+        <v>68.3</v>
+      </c>
+      <c r="D17" s="4">
+        <v>65.3</v>
+      </c>
+      <c r="E17" s="12">
+        <v>213</v>
+      </c>
+      <c r="F17" s="31">
+        <f t="shared" si="0"/>
+        <v>2.9708568943018703</v>
+      </c>
+      <c r="G17" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0868841544607191</v>
+      </c>
+      <c r="H17" s="31">
+        <f t="shared" si="2"/>
+        <v>3.4908418665023402</v>
+      </c>
+      <c r="I17" s="36">
+        <f t="shared" si="3"/>
+        <v>2.9708568943018703</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="4"/>
+        <v>1.0868841544607191</v>
+      </c>
+      <c r="K17" s="37">
+        <f t="shared" si="4"/>
+        <v>3.4908418665023402</v>
+      </c>
+      <c r="L17" s="32">
+        <f t="shared" si="5"/>
+        <v>4.577726020963059</v>
+      </c>
+      <c r="M17" s="45">
+        <f t="shared" si="7"/>
+        <v>54.087732389371489</v>
+      </c>
+      <c r="N17" s="45">
+        <f t="shared" si="6"/>
+        <v>17.502861655766917</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D18" s="4">
+        <v>51.6</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="31">
+        <f t="shared" si="0"/>
+        <v>1.4223575467594609</v>
+      </c>
+      <c r="G18" s="31">
+        <f t="shared" si="1"/>
+        <v>0.85885486018641821</v>
+      </c>
+      <c r="H18" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="32">
+        <f t="shared" si="3"/>
+        <v>1.4223575467594609</v>
+      </c>
+      <c r="J18" s="32">
+        <f t="shared" si="4"/>
+        <v>0.85885486018641821</v>
+      </c>
+      <c r="K18" s="41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="32">
+        <f t="shared" si="5"/>
+        <v>0.85885486018641821</v>
+      </c>
+      <c r="M18" s="45">
+        <f t="shared" si="7"/>
+        <v>-39.617513040716354</v>
+      </c>
+      <c r="N18" s="45">
+        <f t="shared" si="6"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>67.2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>63</v>
+      </c>
+      <c r="E19" s="4">
+        <v>205</v>
+      </c>
+      <c r="F19" s="31">
+        <f t="shared" si="0"/>
+        <v>2.9230100043497176</v>
+      </c>
+      <c r="G19" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0486018641810919</v>
+      </c>
+      <c r="H19" s="31">
+        <f t="shared" si="2"/>
+        <v>3.3597304348966186</v>
+      </c>
+      <c r="I19" s="29">
+        <f t="shared" si="3"/>
+        <v>2.9230100043497176</v>
+      </c>
+      <c r="J19" s="29">
+        <f t="shared" si="4"/>
+        <v>1.0486018641810919</v>
+      </c>
+      <c r="K19" s="29">
+        <f t="shared" si="4"/>
+        <v>3.3597304348966186</v>
+      </c>
+      <c r="L19" s="32">
+        <f t="shared" si="5"/>
+        <v>4.4083322990777107</v>
+      </c>
+      <c r="M19" s="45">
+        <f t="shared" si="7"/>
+        <v>50.814820767554401</v>
+      </c>
+      <c r="N19" s="45">
+        <f t="shared" si="6"/>
+        <v>14.940777824811388</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="D20" s="4">
+        <v>52.2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>61</v>
+      </c>
+      <c r="F20" s="31">
+        <f t="shared" si="0"/>
+        <v>1.017833840800348</v>
+      </c>
+      <c r="G20" s="31">
+        <f t="shared" si="1"/>
+        <v>0.86884154460719043</v>
+      </c>
+      <c r="H20" s="31">
+        <f t="shared" si="2"/>
+        <v>0.99972466599362797</v>
+      </c>
+      <c r="I20" s="29">
+        <f t="shared" si="3"/>
+        <v>1.017833840800348</v>
+      </c>
+      <c r="J20" s="29">
+        <f t="shared" si="3"/>
+        <v>0.86884154460719043</v>
+      </c>
+      <c r="K20" s="29">
+        <f t="shared" si="3"/>
+        <v>0.99972466599362797</v>
+      </c>
+      <c r="L20" s="32">
+        <f t="shared" si="5"/>
+        <v>1.8685662106008185</v>
+      </c>
+      <c r="M20" s="45">
+        <f t="shared" si="7"/>
+        <v>83.582637528687258</v>
+      </c>
+      <c r="N20" s="45">
+        <f t="shared" si="6"/>
+        <v>-1.7791877299422796</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MgSO4, plottet conduktivitet samt tryk
</commit_message>
<xml_diff>
--- a/data/NaCl_IC_analyse_test.xlsx
+++ b/data/NaCl_IC_analyse_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="8_{3C0C4C5D-0172-4F0F-BDE4-87CB5391D010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2687AD11-D3DD-41C7-A971-D690A157CAE7}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="8_{3C0C4C5D-0172-4F0F-BDE4-87CB5391D010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F3602BB9-61E7-410E-83E8-B0713BF2F6AF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A7F57C6-AEBE-42AA-863E-04BDCF82B821}"/>
   </bookViews>
   <sheets>
     <sheet name="NaCl" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="27">
   <si>
     <t>navn</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>deviation charge w/o. SiO2</t>
+  </si>
+  <si>
+    <t>Retentate</t>
   </si>
 </sst>
 </file>
@@ -729,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6429C-0FFF-4E30-BF3A-6A5B96E649C1}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +791,7 @@
         <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -830,7 +833,7 @@
         <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -872,7 +875,7 @@
         <v>125</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,7 +917,7 @@
         <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -942,7 +945,7 @@
         <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -961,7 +964,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="3">
         <v>86</v>
@@ -998,7 +1001,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C18"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1056,7 @@
         <v>220</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1095,7 +1098,7 @@
         <v>248</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,7 +1140,7 @@
         <v>265</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,7 +1182,7 @@
         <v>302</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,7 +1210,7 @@
         <v>329</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1226,7 +1229,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="3">
         <v>178</v>
@@ -1262,7 +1265,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C18"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1320,7 @@
         <v>48.3</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,7 +1362,7 @@
         <v>52.7</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,7 +1404,7 @@
         <v>58.9</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,7 +1446,7 @@
         <v>64.8</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1471,7 +1474,7 @@
         <v>68.3</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,7 +1493,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="4">
         <v>63</v>
@@ -1526,7 +1529,7 @@
   <dimension ref="A1:AP20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,11 +1645,11 @@
         <v>8.4</v>
       </c>
       <c r="F4" s="18">
-        <f t="shared" ref="F4:F20" si="0">C4/$C$1</f>
+        <f>C4/$C$1</f>
         <v>3.5667681600695955</v>
       </c>
       <c r="G4" s="18">
-        <f t="shared" ref="G4:G20" si="1">D4/$D$1</f>
+        <f t="shared" ref="G4:G20" si="0">D4/$D$1</f>
         <v>3.6953455571227076</v>
       </c>
       <c r="H4" s="18">
@@ -1658,7 +1661,7 @@
         <v>3.5667681600695955</v>
       </c>
       <c r="J4" s="21">
-        <f t="shared" ref="J4" si="2">G4*1</f>
+        <f t="shared" ref="J4" si="1">G4*1</f>
         <v>3.6953455571227076</v>
       </c>
       <c r="K4" s="21">
@@ -1718,11 +1721,11 @@
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="32">
+        <f t="shared" ref="F5:F20" si="2">C5/$C$1</f>
+        <v>3.3492822966507179</v>
+      </c>
+      <c r="G5" s="32">
         <f t="shared" si="0"/>
-        <v>3.3492822966507179</v>
-      </c>
-      <c r="G5" s="32">
-        <f t="shared" si="1"/>
         <v>3.3004231311706627</v>
       </c>
       <c r="H5" s="32">
@@ -1794,11 +1797,11 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="25">
+        <f t="shared" si="2"/>
+        <v>3.3492822966507179</v>
+      </c>
+      <c r="G6" s="25">
         <f t="shared" si="0"/>
-        <v>3.3492822966507179</v>
-      </c>
-      <c r="G6" s="25">
-        <f t="shared" si="1"/>
         <v>3.328631875881523</v>
       </c>
       <c r="H6" s="25">
@@ -1869,11 +1872,11 @@
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="28">
+        <f t="shared" si="2"/>
+        <v>2.6533275337103088</v>
+      </c>
+      <c r="G7" s="28">
         <f t="shared" si="0"/>
-        <v>2.6533275337103088</v>
-      </c>
-      <c r="G7" s="28">
-        <f t="shared" si="1"/>
         <v>2.7362482369534553</v>
       </c>
       <c r="H7" s="28">
@@ -1947,11 +1950,11 @@
         <v>31</v>
       </c>
       <c r="F8" s="32">
+        <f t="shared" si="2"/>
+        <v>3.4797738147020447</v>
+      </c>
+      <c r="G8" s="32">
         <f t="shared" si="0"/>
-        <v>3.4797738147020447</v>
-      </c>
-      <c r="G8" s="32">
-        <f t="shared" si="1"/>
         <v>3.3850493653032436</v>
       </c>
       <c r="H8" s="32">
@@ -2023,11 +2026,11 @@
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="25">
+        <f t="shared" si="2"/>
+        <v>3.4797738147020447</v>
+      </c>
+      <c r="G9" s="25">
         <f t="shared" si="0"/>
-        <v>3.4797738147020447</v>
-      </c>
-      <c r="G9" s="25">
-        <f t="shared" si="1"/>
         <v>3.3850493653032436</v>
       </c>
       <c r="H9" s="25">
@@ -2098,11 +2101,11 @@
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="28">
+        <f t="shared" si="2"/>
+        <v>2.7403218790778601</v>
+      </c>
+      <c r="G10" s="28">
         <f t="shared" si="0"/>
-        <v>2.7403218790778601</v>
-      </c>
-      <c r="G10" s="28">
-        <f t="shared" si="1"/>
         <v>2.8208744710860363</v>
       </c>
       <c r="H10" s="28">
@@ -2174,11 +2177,11 @@
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="32">
+        <f t="shared" si="2"/>
+        <v>3.6972596781209224</v>
+      </c>
+      <c r="G11" s="32">
         <f t="shared" si="0"/>
-        <v>3.6972596781209224</v>
-      </c>
-      <c r="G11" s="32">
-        <f t="shared" si="1"/>
         <v>3.5825105782792663</v>
       </c>
       <c r="H11" s="32">
@@ -2222,11 +2225,11 @@
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="25">
+        <f t="shared" si="2"/>
+        <v>3.6972596781209224</v>
+      </c>
+      <c r="G12" s="25">
         <f t="shared" si="0"/>
-        <v>3.6972596781209224</v>
-      </c>
-      <c r="G12" s="25">
-        <f t="shared" si="1"/>
         <v>3.5260930888575457</v>
       </c>
       <c r="H12" s="25">
@@ -2270,11 +2273,11 @@
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="28">
+        <f t="shared" si="2"/>
+        <v>2.8708133971291869</v>
+      </c>
+      <c r="G13" s="28">
         <f t="shared" si="0"/>
-        <v>2.8708133971291869</v>
-      </c>
-      <c r="G13" s="28">
-        <f t="shared" si="1"/>
         <v>2.9619181946403383</v>
       </c>
       <c r="H13" s="28">
@@ -2320,11 +2323,11 @@
         <v>42</v>
       </c>
       <c r="F14" s="32">
+        <f t="shared" si="2"/>
+        <v>3.8712483688560244</v>
+      </c>
+      <c r="G14" s="32">
         <f t="shared" si="0"/>
-        <v>3.8712483688560244</v>
-      </c>
-      <c r="G14" s="32">
-        <f t="shared" si="1"/>
         <v>3.638928067700987</v>
       </c>
       <c r="H14" s="32">
@@ -2396,11 +2399,11 @@
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="25">
+        <f t="shared" si="2"/>
+        <v>3.8277511961722492</v>
+      </c>
+      <c r="G15" s="25">
         <f t="shared" si="0"/>
-        <v>3.8277511961722492</v>
-      </c>
-      <c r="G15" s="25">
-        <f t="shared" si="1"/>
         <v>3.6107193229901267</v>
       </c>
       <c r="H15" s="25">
@@ -2471,11 +2474,11 @@
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="28">
+        <f t="shared" si="2"/>
+        <v>2.9578077424967377</v>
+      </c>
+      <c r="G16" s="28">
         <f t="shared" si="0"/>
-        <v>2.9578077424967377</v>
-      </c>
-      <c r="G16" s="28">
-        <f t="shared" si="1"/>
         <v>3.0747531734837796</v>
       </c>
       <c r="H16" s="28">
@@ -2549,11 +2552,11 @@
         <v>48</v>
       </c>
       <c r="F17" s="32">
+        <f t="shared" si="2"/>
+        <v>3.9582427142235757</v>
+      </c>
+      <c r="G17" s="32">
         <f t="shared" si="0"/>
-        <v>3.9582427142235757</v>
-      </c>
-      <c r="G17" s="32">
-        <f t="shared" si="1"/>
         <v>3.779971791255289</v>
       </c>
       <c r="H17" s="32">
@@ -2625,11 +2628,11 @@
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="28">
+        <f t="shared" si="2"/>
+        <v>3.1317964332318402</v>
+      </c>
+      <c r="G18" s="28">
         <f t="shared" si="0"/>
-        <v>3.1317964332318402</v>
-      </c>
-      <c r="G18" s="28">
-        <f t="shared" si="1"/>
         <v>3.1875881523272214</v>
       </c>
       <c r="H18" s="28">
@@ -2688,7 +2691,7 @@
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>3</v>
@@ -2703,11 +2706,11 @@
         <v>43</v>
       </c>
       <c r="F19" s="32">
+        <f t="shared" si="2"/>
+        <v>3.740756850804698</v>
+      </c>
+      <c r="G19" s="32">
         <f t="shared" si="0"/>
-        <v>3.740756850804698</v>
-      </c>
-      <c r="G19" s="32">
-        <f t="shared" si="1"/>
         <v>3.5825105782792663</v>
       </c>
       <c r="H19" s="32">
@@ -2753,11 +2756,11 @@
         <v>15</v>
       </c>
       <c r="F20" s="28">
+        <f t="shared" si="2"/>
+        <v>2.6098303610265337</v>
+      </c>
+      <c r="G20" s="28">
         <f t="shared" si="0"/>
-        <v>2.6098303610265337</v>
-      </c>
-      <c r="G20" s="28">
-        <f t="shared" si="1"/>
         <v>2.708039492242595</v>
       </c>
       <c r="H20" s="28">
@@ -2803,7 +2806,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3616,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -3725,8 +3728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401685D4-8829-42D7-BB4A-E3F815791FE0}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4602,7 +4605,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>

</xml_diff>